<commit_message>
Correções nas funcionalidades: adicionar, editar, excluir e importar dados no Excel
</commit_message>
<xml_diff>
--- a/dados_lojas.xlsx
+++ b/dados_lojas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E137"/>
+  <dimension ref="A1:E138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3282,6 +3282,33 @@
         </is>
       </c>
     </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>BB</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>1KJ</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>KJ</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>KKJ</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>